<commit_message>
promo banner oxo&hydro country selector oxo
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE14EF2-ABC8-4208-960B-B2FE2957E254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94F3B27F-C29B-41BF-9B5B-C215F57A8A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="11078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="131">
   <si>
     <t>UserName</t>
   </si>
@@ -411,6 +411,15 @@
   </si>
   <si>
     <t>testingqaserdt</t>
+  </si>
+  <si>
+    <t>CountrySelector</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>Japan,United States,Germany,UK,Poland</t>
   </si>
 </sst>
 </file>
@@ -478,7 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -499,6 +508,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -783,91 +796,91 @@
   <dimension ref="A1:BX33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="38" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="6.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="6.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="56.81640625" style="5"/>
-    <col min="29" max="29" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="56.85546875" style="5"/>
+    <col min="29" max="29" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="16384" width="56.81640625" style="5"/>
+    <col min="74" max="74" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -949,7 +962,9 @@
       <c r="AA1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AB1" s="4"/>
+      <c r="AB1" s="4" t="s">
+        <v>129</v>
+      </c>
       <c r="AC1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1095,7 +1110,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1115,7 +1130,7 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
@@ -1138,7 +1153,7 @@
       <c r="V3" s="8"/>
       <c r="W3" s="9"/>
     </row>
-    <row r="4" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1166,7 +1181,7 @@
       <c r="V4" s="8"/>
       <c r="W4" s="9"/>
     </row>
-    <row r="5" spans="1:76" ht="24.7" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1188,7 +1203,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:76" ht="13.55" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:76" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1209,7 +1224,10 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="C7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -1218,8 +1236,12 @@
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="AB7" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A8" s="15"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -1243,12 +1265,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
       <c r="AJ9" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:76" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="AK10" s="2" t="s">
         <v>44</v>
       </c>
@@ -1286,19 +1310,22 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" spans="1:76" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
       <c r="C13" s="6"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="10"/>
@@ -1306,12 +1333,13 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
       <c r="AW14" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.25">
       <c r="AX15" s="5" t="s">
         <v>107</v>
       </c>
@@ -1325,7 +1353,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.25">
       <c r="AX16" s="5" t="s">
         <v>110</v>
       </c>
@@ -1336,12 +1364,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:76" x14ac:dyDescent="0.25">
       <c r="BA17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="3:76" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:76" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C18" s="6"/>
       <c r="Y18" s="3"/>
       <c r="Z18" s="10"/>
@@ -1349,7 +1377,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:76" x14ac:dyDescent="0.25">
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -1359,20 +1387,20 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:76" x14ac:dyDescent="0.25">
       <c r="V20" s="8"/>
       <c r="W20" s="9"/>
     </row>
-    <row r="21" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:76" x14ac:dyDescent="0.25">
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
     </row>
-    <row r="22" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:76" x14ac:dyDescent="0.25">
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="V22" s="11"/>
     </row>
-    <row r="24" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:76" x14ac:dyDescent="0.25">
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="N24" s="6"/>
@@ -1440,7 +1468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:76" x14ac:dyDescent="0.25">
       <c r="C25" s="6"/>
       <c r="E25" s="13"/>
       <c r="F25" s="6"/>
@@ -1448,26 +1476,26 @@
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
     </row>
-    <row r="27" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:76" x14ac:dyDescent="0.25">
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
     </row>
-    <row r="30" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:76" x14ac:dyDescent="0.25">
       <c r="BW30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:76" x14ac:dyDescent="0.25">
       <c r="BW31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="3:76" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:76" x14ac:dyDescent="0.25">
       <c r="BX32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>

</xml_diff>

<commit_message>
oxo minicart helper, testdata,testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C7C934-D15A-4101-92D2-790AF3F4A1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C50D74-D3CD-43C2-A38D-A74BA9BE74F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19220" windowHeight="9580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="167">
   <si>
     <t>UserName</t>
   </si>
@@ -519,6 +519,15 @@
   </si>
   <si>
     <t>My product subscriptions</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>20-Piece POP Container Set</t>
+  </si>
+  <si>
+    <t>Delete Product</t>
   </si>
 </sst>
 </file>
@@ -586,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -613,6 +622,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -896,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,7 +934,7 @@
     <col min="17" max="17" width="10.54296875" style="15" customWidth="1"/>
     <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24.08984375" style="5" customWidth="1"/>
@@ -1588,6 +1602,12 @@
       </c>
     </row>
     <row r="16" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="T16" s="20">
+        <v>3</v>
+      </c>
       <c r="BF16" s="5" t="s">
         <v>110</v>
       </c>
@@ -1598,12 +1618,18 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="T17" s="19" t="s">
+        <v>165</v>
+      </c>
       <c r="BI17" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="7:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="G18" s="6"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="10"/>
@@ -1611,7 +1637,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1621,22 +1647,22 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
     </row>
-    <row r="21" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1705,7 +1731,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1714,22 +1740,22 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="27" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CE30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CE31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="7:84" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CF32" s="5" t="s">
         <v>102</v>
       </c>

</xml_diff>

<commit_message>
warning messages for admin helper and oxo test data
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C50D74-D3CD-43C2-A38D-A74BA9BE74F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B401FF-1443-4B2C-BC43-82190F23203C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19220" windowHeight="9580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="168">
   <si>
     <t>UserName</t>
   </si>
@@ -528,6 +528,9 @@
   </si>
   <si>
     <t>Delete Product</t>
+  </si>
+  <si>
+    <t>Shipping Issues,Cooking &amp; Baking,Baby &amp; Toddler</t>
   </si>
 </sst>
 </file>
@@ -911,98 +914,98 @@
   <dimension ref="A1:CF33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="80.81640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.1796875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="15" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.08984375" style="5" customWidth="1"/>
-    <col min="24" max="24" width="20.6328125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="24.140625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="5" customWidth="1"/>
     <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.26953125" style="15" customWidth="1"/>
-    <col min="35" max="35" width="56.81640625" style="5"/>
-    <col min="36" max="36" width="56.81640625" style="15"/>
-    <col min="37" max="37" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36.28515625" style="15" customWidth="1"/>
+    <col min="35" max="35" width="56.85546875" style="5"/>
+    <col min="36" max="36" width="56.85546875" style="15"/>
+    <col min="37" max="37" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="56.81640625" style="5"/>
+    <col min="82" max="82" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1267,7 +1270,7 @@
       <c r="F2" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="6"/>
+      <c r="G2" s="17"/>
       <c r="H2" s="5" t="s">
         <v>133</v>
       </c>
@@ -1310,7 +1313,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
@@ -1335,7 +1338,7 @@
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1368,7 +1371,7 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
     </row>
-    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1395,7 +1398,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1417,7 +1420,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>128</v>
       </c>
@@ -1440,13 +1443,13 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>130</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="17" t="s">
-        <v>132</v>
+        <v>167</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
@@ -1469,7 +1472,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>145</v>
       </c>
@@ -1480,7 +1483,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>146</v>
       </c>
@@ -1532,7 +1535,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>147</v>
       </c>
@@ -1544,7 +1547,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>148</v>
       </c>
@@ -1556,7 +1559,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>149</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>150</v>
       </c>
@@ -1581,7 +1584,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>155</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>164</v>
       </c>
@@ -1618,7 +1621,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>166</v>
       </c>
@@ -1629,7 +1632,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G18" s="6"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="10"/>
@@ -1637,7 +1640,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
@@ -1647,22 +1650,22 @@
         <v>342</v>
       </c>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1731,7 +1734,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1740,27 +1743,27 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
       <c r="CE30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.25">
       <c r="CE31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
       <c r="CF32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>

</xml_diff>

<commit_message>
OXO - 2 checkout test cases commit Helper,testcase,testdata, Admin TestNg files commit.
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B401FF-1443-4B2C-BC43-82190F23203C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79A046-6868-4053-91D9-5A0056E8B324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
   <si>
     <t>UserName</t>
   </si>
@@ -531,6 +531,15 @@
   </si>
   <si>
     <t>Shipping Issues,Cooking &amp; Baking,Baby &amp; Toddler</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Pet POP Container (5.8 Qt.)</t>
+  </si>
+  <si>
+    <t>Lotuswave@123</t>
   </si>
 </sst>
 </file>
@@ -913,99 +922,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="80.85546875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="80.81640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" style="15" customWidth="1"/>
+    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="24.1796875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="20.54296875" style="5" customWidth="1"/>
     <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.28515625" style="15" customWidth="1"/>
-    <col min="35" max="35" width="56.85546875" style="5"/>
-    <col min="36" max="36" width="56.85546875" style="15"/>
-    <col min="37" max="37" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36.26953125" style="15" customWidth="1"/>
+    <col min="35" max="35" width="56.81640625" style="5"/>
+    <col min="36" max="36" width="56.81640625" style="15"/>
+    <col min="37" max="37" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="56.85546875" style="5"/>
+    <col min="82" max="82" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1270,7 +1279,9 @@
       <c r="F2" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="G2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>170</v>
+      </c>
       <c r="H2" s="5" t="s">
         <v>133</v>
       </c>
@@ -1313,7 +1324,7 @@
         <v>9898989898</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>112</v>
       </c>
@@ -1338,7 +1349,7 @@
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>117</v>
       </c>
@@ -1371,7 +1382,7 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
     </row>
-    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>125</v>
       </c>
@@ -1398,7 +1409,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>126</v>
       </c>
@@ -1420,7 +1431,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>128</v>
       </c>
@@ -1443,7 +1454,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>130</v>
       </c>
@@ -1472,7 +1483,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>145</v>
       </c>
@@ -1483,7 +1494,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>146</v>
       </c>
@@ -1535,7 +1546,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>147</v>
       </c>
@@ -1547,7 +1558,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>148</v>
       </c>
@@ -1559,7 +1570,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>149</v>
       </c>
@@ -1573,7 +1584,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>150</v>
       </c>
@@ -1584,7 +1595,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>155</v>
       </c>
@@ -1604,7 +1615,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>164</v>
       </c>
@@ -1621,7 +1632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>166</v>
       </c>
@@ -1632,40 +1643,44 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
+        <v>168</v>
+      </c>
       <c r="G18" s="6"/>
+      <c r="T18" s="5" t="s">
+        <v>169</v>
+      </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="10"/>
       <c r="AK18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="A19" s="15"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="AE19" s="1"/>
-      <c r="AK19" s="5">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
@@ -1734,7 +1749,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1743,27 +1758,27 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CE30" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CE31" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
       <c r="CF32" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:13" x14ac:dyDescent="0.35">
       <c r="G33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -1781,8 +1796,9 @@
     <hyperlink ref="J2" r:id="rId8" xr:uid="{09DDF643-6769-411C-9C0A-0F3FFD7CCB83}"/>
     <hyperlink ref="F2" r:id="rId9" xr:uid="{79A5204C-1E5E-4D7D-BE23-3D875D65F089}"/>
     <hyperlink ref="AH7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
+    <hyperlink ref="G2" r:id="rId11" xr:uid="{6BA18CB7-8C64-4E80-8B31-7A3FF7879487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
oxo Guest user checkout for both preprod and stage environment
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B79A046-6868-4053-91D9-5A0056E8B324}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145475E1-7CE5-4ECD-B26E-A9D5C6AB7614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="177">
   <si>
     <t>UserName</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t>cardNumber</t>
-  </si>
-  <si>
-    <t>ExpYear</t>
   </si>
   <si>
     <t>ExpMonth</t>
@@ -540,6 +537,27 @@
   </si>
   <si>
     <t>Lotuswave@123</t>
+  </si>
+  <si>
+    <t>addproduct</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>PaymentDetails</t>
+  </si>
+  <si>
+    <t>4242424242424242</t>
+  </si>
+  <si>
+    <t>ExpMonthYear</t>
+  </si>
+  <si>
+    <t>03/30</t>
+  </si>
+  <si>
+    <t>9-Cup Coffee Maker</t>
   </si>
 </sst>
 </file>
@@ -607,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -639,6 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -922,99 +941,99 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T19" sqref="T19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="80.81640625" style="15" customWidth="1"/>
-    <col min="6" max="6" width="30.7265625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.1796875" style="15" customWidth="1"/>
-    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.54296875" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="15" customWidth="1"/>
+    <col min="5" max="5" width="80.85546875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="15" customWidth="1"/>
+    <col min="11" max="11" width="30.7109375" style="5" customWidth="1"/>
+    <col min="12" max="12" width="54.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="15" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.1796875" style="5" customWidth="1"/>
-    <col min="24" max="24" width="20.54296875" style="5" customWidth="1"/>
+    <col min="23" max="23" width="24.140625" style="5" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="5" customWidth="1"/>
     <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.26953125" style="15" customWidth="1"/>
-    <col min="35" max="35" width="56.81640625" style="5"/>
-    <col min="36" max="36" width="56.81640625" style="15"/>
-    <col min="37" max="37" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36.28515625" style="15" customWidth="1"/>
+    <col min="35" max="35" width="56.85546875" style="5"/>
+    <col min="36" max="36" width="56.85546875" style="15"/>
+    <col min="37" max="37" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="56.81640625" style="5"/>
+    <col min="82" max="82" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="16384" width="56.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1022,16 +1041,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>1</v>
@@ -1043,43 +1062,43 @@
         <v>5</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L1" s="16" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="S1" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="T1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>20</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>6</v>
@@ -1088,13 +1107,13 @@
         <v>7</v>
       </c>
       <c r="Y1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="AA1" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AB1" s="4" t="s">
         <v>8</v>
@@ -1109,166 +1128,166 @@
         <v>11</v>
       </c>
       <c r="AF1" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="AI1" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="AK1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AH1" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="AK1" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="AL1" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AM1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AN1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AO1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AO1" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="AP1" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AQ1" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AT1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AU1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AV1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AX1" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="AY1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="BC1" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BD1" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BE1" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="BF1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BG1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BH1" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="BI1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BJ1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="BK1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CD1" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="CE1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="CF1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="CF1" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1277,22 +1296,22 @@
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H2" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>134</v>
-      </c>
       <c r="J2" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
@@ -1300,43 +1319,46 @@
       <c r="O2" s="6"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="T2" s="6"/>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="X2" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB2" s="11" t="s">
         <v>137</v>
-      </c>
-      <c r="AB2" s="11" t="s">
-        <v>138</v>
       </c>
       <c r="AC2" s="5">
         <v>9898989898</v>
       </c>
     </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
       <c r="N3" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
@@ -1349,26 +1371,26 @@
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
     </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L4" s="6"/>
       <c r="M4" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="N4" s="7"/>
       <c r="O4" s="6"/>
@@ -1382,26 +1404,26 @@
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
     </row>
-    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L5" s="6"/>
       <c r="M5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AE5" s="1"/>
       <c r="AF5" s="10"/>
@@ -1409,17 +1431,17 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1431,9 +1453,9 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" s="6"/>
       <c r="K7" s="6"/>
@@ -1445,62 +1467,62 @@
       <c r="Q7" s="17"/>
       <c r="R7" s="6"/>
       <c r="AH7" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="AI7" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="AJ7" s="17" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>129</v>
-      </c>
-      <c r="AJ7" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
-        <v>130</v>
       </c>
       <c r="K8" s="6"/>
       <c r="L8" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="AL8" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="AM8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AN8" s="5">
         <v>123456</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AP8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AQ8" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR9" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>145</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="AR9" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>146</v>
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
@@ -1510,72 +1532,72 @@
       <c r="AH10" s="14"/>
       <c r="AJ10" s="14"/>
       <c r="AS10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AT10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AU10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AV10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX10" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="AU10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV10" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AW10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX10" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="AY10" s="2">
         <v>27</v>
       </c>
       <c r="AZ10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="BA10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BB10" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="BB10" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="BC10" s="2">
         <v>2</v>
       </c>
       <c r="BD10" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G13" s="6"/>
       <c r="AE13" s="1"/>
@@ -1584,72 +1606,72 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BE14" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BF15" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BH15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BH15" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="BI15" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="T16" s="20">
         <v>3</v>
       </c>
       <c r="BF16" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BG16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="BG16" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="BH16" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="T17" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BI17" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G18" s="6"/>
       <c r="T18" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="AE18" s="3"/>
       <c r="AF18" s="10"/>
@@ -1657,54 +1679,71 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="A19" s="15"/>
+    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>170</v>
+      </c>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
+      <c r="T19" s="5" t="s">
+        <v>176</v>
+      </c>
       <c r="AE19" s="1"/>
     </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>172</v>
+      </c>
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
-    </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.35">
+      <c r="AE20" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="AF20" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="AK20" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
       <c r="BJ24" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="BK24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BL24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BL24" s="5" t="s">
+      <c r="BM24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="BO24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BM24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BN24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="BO24" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="BP24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="BQ24" s="5">
         <v>9</v>
@@ -1713,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="BS24" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="BT24" s="12">
         <v>40000</v>
@@ -1725,31 +1764,31 @@
         <v>1000000</v>
       </c>
       <c r="BW24" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="BX24" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BY24" s="5">
         <v>57501</v>
       </c>
       <c r="BZ24" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="CA24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="CD24" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="CC24" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="CD24" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1758,27 +1797,27 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
       <c r="CE30" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="CE31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.35">
-      <c r="CE31" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
       <c r="CF32" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
       <c r="G33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>

</xml_diff>

<commit_message>
OXO 1  testcase commit, testcase, helper,estdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145475E1-7CE5-4ECD-B26E-A9D5C6AB7614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34237B3E-5D03-4C2A-9526-FE6F355A4A01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19200" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="180">
   <si>
     <t>UserName</t>
   </si>
@@ -558,6 +558,15 @@
   </si>
   <si>
     <t>9-Cup Coffee Maker</t>
+  </si>
+  <si>
+    <t>Shippingmethods</t>
+  </si>
+  <si>
+    <t>Ground</t>
+  </si>
+  <si>
+    <t>United State</t>
   </si>
 </sst>
 </file>
@@ -939,101 +948,102 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CF33"/>
+  <dimension ref="A1:CG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="80.85546875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" style="15" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" style="5" customWidth="1"/>
-    <col min="12" max="12" width="54.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="96.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="15" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7265625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="80.81640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="30.7265625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.1796875" style="15" customWidth="1"/>
+    <col min="11" max="11" width="30.7265625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.54296875" style="15" customWidth="1"/>
+    <col min="18" max="18" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.140625" style="5" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" style="5" customWidth="1"/>
-    <col min="25" max="25" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.1796875" style="5" customWidth="1"/>
+    <col min="24" max="24" width="20.54296875" style="5" customWidth="1"/>
+    <col min="25" max="25" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36.28515625" style="15" customWidth="1"/>
-    <col min="35" max="35" width="56.85546875" style="5"/>
-    <col min="36" max="36" width="56.85546875" style="15"/>
-    <col min="37" max="37" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="11.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="161.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="9.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="4.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="20.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="35.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="146.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="28.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="43.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="8.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="6.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="12.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="12.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="6.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="7.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="18.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="16384" width="56.85546875" style="5"/>
+    <col min="30" max="30" width="11" style="15" customWidth="1"/>
+    <col min="31" max="31" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="36.26953125" style="15" customWidth="1"/>
+    <col min="36" max="36" width="56.81640625" style="5"/>
+    <col min="37" max="37" width="56.81640625" style="15"/>
+    <col min="38" max="38" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1122,172 +1132,175 @@
         <v>9</v>
       </c>
       <c r="AD1" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="AE1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AL1" s="5" t="s">
+      <c r="AM1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CE1" s="5" t="s">
+      <c r="CF1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CG1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1336,6 +1349,12 @@
       <c r="X2" s="5" t="s">
         <v>136</v>
       </c>
+      <c r="Y2" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="AA2" s="5" t="s">
         <v>171</v>
       </c>
@@ -1345,8 +1364,11 @@
       <c r="AC2" s="5">
         <v>9898989898</v>
       </c>
-    </row>
-    <row r="3" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="AD2" s="15" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>111</v>
       </c>
@@ -1370,8 +1392,9 @@
       <c r="V3" s="6"/>
       <c r="AB3" s="8"/>
       <c r="AC3" s="9"/>
-    </row>
-    <row r="4" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="AD3" s="9"/>
+    </row>
+    <row r="4" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>116</v>
       </c>
@@ -1403,8 +1426,9 @@
       <c r="V4" s="6"/>
       <c r="AB4" s="8"/>
       <c r="AC4" s="9"/>
-    </row>
-    <row r="5" spans="1:84" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD4" s="9"/>
+    </row>
+    <row r="5" spans="1:85" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>124</v>
       </c>
@@ -1425,13 +1449,13 @@
       <c r="M5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="10"/>
-      <c r="AK5" s="9">
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="10"/>
+      <c r="AL5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:84" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:85" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>125</v>
       </c>
@@ -1453,7 +1477,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>127</v>
       </c>
@@ -1466,17 +1490,17 @@
       <c r="P7" s="6"/>
       <c r="Q7" s="17"/>
       <c r="R7" s="6"/>
-      <c r="AH7" s="17" t="s">
+      <c r="AI7" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="AI7" s="5" t="s">
+      <c r="AJ7" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AJ7" s="17" t="s">
+      <c r="AK7" s="17" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="8" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>129</v>
       </c>
@@ -1486,37 +1510,37 @@
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="AL8" s="5" t="s">
+      <c r="AM8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AM8" s="5" t="s">
+      <c r="AN8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AN8" s="5">
+      <c r="AO8" s="5">
         <v>123456</v>
       </c>
-      <c r="AO8" s="5" t="s">
+      <c r="AP8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AP8" s="5" t="s">
+      <c r="AQ8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="5" t="s">
+      <c r="AR8" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>144</v>
       </c>
       <c r="D9" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="AR9" s="5" t="s">
+      <c r="AS9" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:84" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>145</v>
       </c>
@@ -1529,46 +1553,47 @@
       <c r="J10" s="14"/>
       <c r="L10" s="14"/>
       <c r="Q10" s="14"/>
-      <c r="AH10" s="14"/>
-      <c r="AJ10" s="14"/>
-      <c r="AS10" s="2" t="s">
+      <c r="AD10" s="14"/>
+      <c r="AI10" s="14"/>
+      <c r="AK10" s="14"/>
+      <c r="AT10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AT10" s="2" t="s">
+      <c r="AU10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AU10" s="2" t="s">
+      <c r="AV10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AV10" s="2" t="s">
+      <c r="AW10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AW10" s="2" t="s">
+      <c r="AX10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AX10" s="2" t="s">
+      <c r="AY10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AY10" s="2">
+      <c r="AZ10" s="2">
         <v>27</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BA10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BB10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="BC10" s="2">
+      <c r="BD10" s="2">
         <v>2</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="BE10" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>146</v>
       </c>
@@ -1580,7 +1605,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>147</v>
       </c>
@@ -1592,7 +1617,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>148</v>
       </c>
@@ -1600,72 +1625,72 @@
         <v>153</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="10"/>
-      <c r="AK13" s="9">
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="10"/>
+      <c r="AL13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>149</v>
       </c>
       <c r="E14" t="s">
         <v>131</v>
       </c>
-      <c r="BE14" s="5" t="s">
+      <c r="BF14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>154</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="BF15" s="5" t="s">
+      <c r="BG15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BH15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BH15" s="5" t="s">
+      <c r="BI15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BI15" s="6" t="s">
+      <c r="BJ15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>163</v>
       </c>
       <c r="T16" s="20">
         <v>3</v>
       </c>
-      <c r="BF16" s="5" t="s">
+      <c r="BG16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BG16" s="5" t="s">
+      <c r="BH16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="BH16" s="6" t="s">
+      <c r="BI16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>165</v>
       </c>
       <c r="T17" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="BI17" s="5" t="s">
+      <c r="BJ17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:84" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>167</v>
       </c>
@@ -1673,13 +1698,13 @@
       <c r="T18" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="10"/>
-      <c r="AK18" s="9">
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="10"/>
+      <c r="AL18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>170</v>
       </c>
@@ -1690,105 +1715,106 @@
       <c r="T19" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="AE19" s="1"/>
-    </row>
-    <row r="20" spans="1:84" x14ac:dyDescent="0.25">
+      <c r="AF19" s="1"/>
+    </row>
+    <row r="20" spans="1:85" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>172</v>
       </c>
       <c r="AB20" s="8"/>
       <c r="AC20" s="9"/>
-      <c r="AE20" s="11" t="s">
+      <c r="AD20" s="9"/>
+      <c r="AF20" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="AF20" s="21" t="s">
+      <c r="AG20" s="21" t="s">
         <v>175</v>
       </c>
-      <c r="AK20" s="5">
+      <c r="AL20" s="5">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:85" x14ac:dyDescent="0.35">
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
     </row>
-    <row r="22" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:85" x14ac:dyDescent="0.35">
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="AB22" s="11"/>
     </row>
-    <row r="24" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:85" x14ac:dyDescent="0.35">
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="BJ24" s="5" t="s">
+      <c r="BK24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BK24" s="5" t="s">
+      <c r="BL24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BL24" s="5" t="s">
+      <c r="BM24" s="5" t="s">
         <v>72</v>
-      </c>
-      <c r="BM24" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="BN24" s="5" t="s">
         <v>44</v>
       </c>
       <c r="BO24" s="5" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="BP24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BQ24" s="5">
+      <c r="BQ24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="BR24" s="5">
         <v>9</v>
       </c>
-      <c r="BR24" s="5">
+      <c r="BS24" s="5">
         <v>10</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BT24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BT24" s="12">
+      <c r="BU24" s="12">
         <v>40000</v>
       </c>
-      <c r="BU24" s="5">
+      <c r="BV24" s="5">
         <v>12</v>
       </c>
-      <c r="BV24" s="12">
+      <c r="BW24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BX24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BY24" s="5">
+      <c r="BZ24" s="5">
         <v>57501</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CB24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:85" x14ac:dyDescent="0.35">
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1797,27 +1823,27 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
     </row>
-    <row r="27" spans="1:84" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:85" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="CE30" s="5" t="s">
+    <row r="30" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CF30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="CE31" s="5" t="s">
+    <row r="31" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CF31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:84" x14ac:dyDescent="0.25">
-      <c r="CF32" s="5" t="s">
+    <row r="32" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="CG32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="7:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:13" x14ac:dyDescent="0.35">
       <c r="G33" s="6"/>
       <c r="K33" s="6"/>
       <c r="L33" s="6"/>
@@ -1825,7 +1851,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BI15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BJ15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
@@ -1834,7 +1860,7 @@
     <hyperlink ref="K2" r:id="rId7" xr:uid="{A3F582FF-4788-4DAE-ABAC-5439277BD83D}"/>
     <hyperlink ref="J2" r:id="rId8" xr:uid="{09DDF643-6769-411C-9C0A-0F3FFD7CCB83}"/>
     <hyperlink ref="F2" r:id="rId9" xr:uid="{79A5204C-1E5E-4D7D-BE23-3D875D65F089}"/>
-    <hyperlink ref="AH7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
+    <hyperlink ref="AI7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
     <hyperlink ref="G2" r:id="rId11" xr:uid="{6BA18CB7-8C64-4E80-8B31-7A3FF7879487}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
oxo minicart scroll helper,testdata and testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58CCC56-24AD-4A84-9850-0AC222C432C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14EF5F9-CA75-48CE-9405-1F56228507FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="2160" windowWidth="15360" windowHeight="7155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="185">
   <si>
     <t>UserName</t>
   </si>
@@ -567,6 +567,21 @@
   </si>
   <si>
     <t>United State</t>
+  </si>
+  <si>
+    <t>Soap Dispensing Dish Brush Refills (2pk.)</t>
+  </si>
+  <si>
+    <t>8-Piece POP Container Baking Set</t>
+  </si>
+  <si>
+    <t>pop products</t>
+  </si>
+  <si>
+    <t>searchproduct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Space Saving Drying Rack </t>
   </si>
 </sst>
 </file>
@@ -950,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="N4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,8 +989,8 @@
     <col min="17" max="17" width="10.5703125" style="15" customWidth="1"/>
     <col min="18" max="18" width="19.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="38.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" style="5" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="24.140625" style="5" customWidth="1"/>
     <col min="24" max="24" width="20.5703125" style="5" customWidth="1"/>
@@ -1735,14 +1750,29 @@
       </c>
     </row>
     <row r="21" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>182</v>
+      </c>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
+      <c r="T21" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="U21" s="15" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="22" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>183</v>
+      </c>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
+      <c r="T22" s="15" t="s">
+        <v>184</v>
+      </c>
       <c r="AB22" s="11"/>
     </row>
     <row r="24" spans="1:85" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
OXO, HF - 36, 37 testcases commit- testcases, testdata, helper
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="26" documentId="13_ncr:1_{A14EF5F9-CA75-48CE-9405-1F56228507FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE6390B6-526A-4971-8134-6E30EF9B8CBE}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{A14EF5F9-CA75-48CE-9405-1F56228507FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F27A80AF-40A5-48F1-9B64-215634BFB292}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19180" windowHeight="9120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14220" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="195">
   <si>
     <t>UserName</t>
   </si>
@@ -606,6 +606,12 @@
   </si>
   <si>
     <t>gfdfdg</t>
+  </si>
+  <si>
+    <t>shippingpagerrormsg</t>
+  </si>
+  <si>
+    <t>firstname,lastname,street,city,region,postcode,telephone</t>
   </si>
 </sst>
 </file>
@@ -989,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CG33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1852,7 +1858,12 @@
       </c>
     </row>
     <row r="24" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="K24" s="6"/>
+      <c r="A24" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>194</v>
+      </c>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>

</xml_diff>

<commit_message>
OXO,HF helpers, new unit test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="28" documentId="13_ncr:1_{A14EF5F9-CA75-48CE-9405-1F56228507FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F27A80AF-40A5-48F1-9B64-215634BFB292}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9B65D9-6073-463A-A0F6-7BFCE6907700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14220" windowHeight="6470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19220" windowHeight="9580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="200">
   <si>
     <t>UserName</t>
   </si>
@@ -612,6 +612,21 @@
   </si>
   <si>
     <t>firstname,lastname,street,city,region,postcode,telephone</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Discountcode</t>
+  </si>
+  <si>
+    <t>InvalidDiscountcode</t>
+  </si>
+  <si>
+    <t>GGQA$25</t>
+  </si>
+  <si>
+    <t>GGQA$255</t>
   </si>
 </sst>
 </file>
@@ -679,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -712,6 +727,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -993,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CG33"/>
+  <dimension ref="A1:CI33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="BE7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BF25" sqref="BF25:BG25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,38 +1074,39 @@
     <col min="55" max="55" width="20.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="16384" width="56.81640625" style="5"/>
+    <col min="58" max="59" width="35.453125" style="15" customWidth="1"/>
+    <col min="60" max="60" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1260,92 +1278,98 @@
       <c r="BE1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BF1" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="BG1" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="BH1" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="CF1" s="5" t="s">
+      <c r="CH1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="CG1" s="5" t="s">
+      <c r="CI1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1413,7 +1437,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>111</v>
       </c>
@@ -1445,7 +1469,7 @@
       <c r="AC3" s="9"/>
       <c r="AD3" s="9"/>
     </row>
-    <row r="4" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>116</v>
       </c>
@@ -1485,7 +1509,7 @@
       <c r="AC4" s="9"/>
       <c r="AD4" s="9"/>
     </row>
-    <row r="5" spans="1:85" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:87" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>123</v>
       </c>
@@ -1520,7 +1544,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:85" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:87" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>124</v>
       </c>
@@ -1542,7 +1566,7 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
     </row>
-    <row r="7" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>126</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>128</v>
       </c>
@@ -1594,7 +1618,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>143</v>
       </c>
@@ -1605,7 +1629,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:85" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:87" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>144</v>
       </c>
@@ -1657,8 +1681,10 @@
       <c r="BE10" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="BF10" s="14"/>
+      <c r="BG10" s="14"/>
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>145</v>
       </c>
@@ -1670,7 +1696,7 @@
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
     </row>
-    <row r="12" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>146</v>
       </c>
@@ -1682,7 +1708,7 @@
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
     </row>
-    <row r="13" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>147</v>
       </c>
@@ -1696,66 +1722,66 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>148</v>
       </c>
       <c r="E14" t="s">
         <v>130</v>
       </c>
-      <c r="BF14" s="5" t="s">
+      <c r="BH14" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>153</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="BG15" s="5" t="s">
+      <c r="BI15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BH15" s="5" t="s">
+      <c r="BJ15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BI15" s="5" t="s">
+      <c r="BK15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BJ15" s="6" t="s">
+      <c r="BL15" s="6" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>162</v>
       </c>
       <c r="T16" s="20">
         <v>3</v>
       </c>
-      <c r="BG16" s="5" t="s">
+      <c r="BI16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BH16" s="5" t="s">
+      <c r="BJ16" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="BI16" s="6" t="s">
+      <c r="BK16" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>164</v>
       </c>
       <c r="T17" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="BJ17" s="5" t="s">
+      <c r="BL17" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:85" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:87" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>166</v>
       </c>
@@ -1769,7 +1795,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>169</v>
       </c>
@@ -1782,7 +1808,7 @@
       </c>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>171</v>
       </c>
@@ -1799,7 +1825,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>181</v>
       </c>
@@ -1813,7 +1839,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>182</v>
       </c>
@@ -1825,7 +1851,7 @@
       </c>
       <c r="AB22" s="11"/>
     </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>184</v>
       </c>
@@ -1857,7 +1883,7 @@
         <v>6546466555</v>
       </c>
     </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:87" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>193</v>
       </c>
@@ -1867,71 +1893,74 @@
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="T24" s="6"/>
-      <c r="BK24" s="5" t="s">
+      <c r="BM24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BL24" s="5" t="s">
+      <c r="BN24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BM24" s="5" t="s">
+      <c r="BO24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BN24" s="5" t="s">
+      <c r="BP24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BO24" s="5" t="s">
+      <c r="BQ24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="BP24" s="5" t="s">
+      <c r="BR24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BS24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BR24" s="5">
+      <c r="BT24" s="5">
         <v>9</v>
       </c>
-      <c r="BS24" s="5">
+      <c r="BU24" s="5">
         <v>10</v>
       </c>
-      <c r="BT24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="BU24" s="12">
+      <c r="BW24" s="12">
         <v>40000</v>
       </c>
-      <c r="BV24" s="5">
+      <c r="BX24" s="5">
         <v>12</v>
       </c>
-      <c r="BW24" s="12">
+      <c r="BY24" s="12">
         <v>1000000</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="BZ24" s="5">
+      <c r="CB24" s="5">
         <v>57501</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CC24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CB24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CE24" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CF24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="CE24" s="5" t="s">
+      <c r="CG24" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="25" spans="1:85" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:87" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>195</v>
+      </c>
       <c r="G25" s="6"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
@@ -1939,24 +1968,30 @@
       <c r="L25" s="6"/>
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-    </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.35">
+      <c r="BF25" s="23" t="s">
+        <v>198</v>
+      </c>
+      <c r="BG25" s="23" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:87" x14ac:dyDescent="0.35">
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
       <c r="M27" s="6"/>
     </row>
-    <row r="30" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="CF30" s="5" t="s">
+    <row r="30" spans="1:87" x14ac:dyDescent="0.35">
+      <c r="CH30" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="CF31" s="5" t="s">
+    <row r="31" spans="1:87" x14ac:dyDescent="0.35">
+      <c r="CH31" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="32" spans="1:85" x14ac:dyDescent="0.35">
-      <c r="CG32" s="5" t="s">
+    <row r="32" spans="1:87" x14ac:dyDescent="0.35">
+      <c r="CI32" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1968,7 +2003,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BJ15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BL15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="B5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="K6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="K5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>

</xml_diff>

<commit_message>
OXO-change email testcase,helper,testdata,HF XML
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FF556A-22CF-4615-86A1-A7513EFE701B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7F4C23-FCEF-4B42-8853-924BBEFC1435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="228">
   <si>
     <t>UserName</t>
   </si>
@@ -693,6 +693,33 @@
 United States
 9898989898</t>
   </si>
+  <si>
+    <t>CurrentPassword</t>
+  </si>
+  <si>
+    <t>Newpassword</t>
+  </si>
+  <si>
+    <t>Qatest@123</t>
+  </si>
+  <si>
+    <t>NonmatchPassword</t>
+  </si>
+  <si>
+    <t>InvalidnewPassword</t>
+  </si>
+  <si>
+    <t>passworderror</t>
+  </si>
+  <si>
+    <t>Password confirmation doesn't match entered password.</t>
+  </si>
+  <si>
+    <t>Minimum length of this field must be equal or greater than 8 symbols. Leading and trailing spaces will be ignored.</t>
+  </si>
+  <si>
+    <t>The password doesn't match this account. Verify the password and try again.</t>
+  </si>
 </sst>
 </file>
 
@@ -701,7 +728,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,6 +754,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -759,7 +792,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -798,6 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1079,10 +1113,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CL33"/>
+  <dimension ref="A1:CQ33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AG27" sqref="AG27"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1092,91 +1126,92 @@
     <col min="5" max="5" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="30.7265625" style="15" customWidth="1"/>
     <col min="8" max="8" width="80.81640625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="30.7265625" style="15" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.1796875" style="15" customWidth="1"/>
-    <col min="14" max="14" width="30.7265625" style="5" customWidth="1"/>
-    <col min="15" max="15" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.54296875" style="15" customWidth="1"/>
-    <col min="21" max="21" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="24.1796875" style="5" customWidth="1"/>
-    <col min="27" max="27" width="20.54296875" style="5" customWidth="1"/>
-    <col min="28" max="28" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11" style="15" customWidth="1"/>
-    <col min="34" max="34" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="36.26953125" style="15" customWidth="1"/>
-    <col min="39" max="39" width="56.81640625" style="5"/>
-    <col min="40" max="40" width="56.81640625" style="15"/>
-    <col min="41" max="41" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="35.453125" style="15" customWidth="1"/>
-    <col min="63" max="63" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="91" max="16384" width="56.81640625" style="5"/>
+    <col min="9" max="11" width="30.7265625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.1796875" style="15" customWidth="1"/>
+    <col min="16" max="16" width="30.7265625" style="5" customWidth="1"/>
+    <col min="17" max="17" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="54.81640625" style="15" customWidth="1"/>
+    <col min="21" max="21" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.54296875" style="15" customWidth="1"/>
+    <col min="26" max="26" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="30.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.1796875" style="5" customWidth="1"/>
+    <col min="32" max="32" width="20.54296875" style="5" customWidth="1"/>
+    <col min="33" max="33" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11" style="15" customWidth="1"/>
+    <col min="39" max="39" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="10" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="36.26953125" style="15" customWidth="1"/>
+    <col min="44" max="44" width="56.81640625" style="5"/>
+    <col min="45" max="45" width="56.81640625" style="15"/>
+    <col min="46" max="46" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="161.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="4.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="20.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="35.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="35.453125" style="15" customWidth="1"/>
+    <col min="68" max="68" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="6.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="15.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="17" style="5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="11.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="7.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="14" style="5" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="5" style="5" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="10.453125" style="5" bestFit="1" customWidth="1"/>
+    <col min="96" max="16384" width="56.81640625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1204,251 +1239,266 @@
       <c r="I1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="22" t="s">
+        <v>222</v>
+      </c>
+      <c r="S1" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="U1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AP1" s="5" t="s">
+      <c r="AU1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AX1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AU1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BI1" s="22" t="s">
+      <c r="BN1" s="22" t="s">
         <v>195</v>
       </c>
-      <c r="BJ1" s="22" t="s">
+      <c r="BO1" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BR1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CK1" s="5" t="s">
+      <c r="CP1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="CL1" s="5" t="s">
+      <c r="CQ1" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -1468,96 +1518,104 @@
       <c r="I2" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17" t="s">
         <v>167</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="5" t="s">
+      <c r="Y2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="AE2" s="11" t="s">
+      <c r="AJ2" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="AF2" s="5">
+      <c r="AK2" s="5">
         <v>9898989898</v>
       </c>
-      <c r="AG2" s="15" t="s">
+      <c r="AL2" s="15" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>110</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="15" t="s">
+      <c r="L3" s="6"/>
+      <c r="M3" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="N3" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
       <c r="P3" s="6"/>
-      <c r="Q3" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
       <c r="T3" s="17"/>
       <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
+      <c r="V3" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="AE3" s="8"/>
-      <c r="AF3" s="9"/>
-      <c r="AG3" s="9"/>
-    </row>
-    <row r="4" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="Y3" s="17"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" s="6"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
+    </row>
+    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>115</v>
       </c>
@@ -1568,36 +1626,41 @@
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="M4" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="N4" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="O4" s="6"/>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="6"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
+      <c r="V4" s="7"/>
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="AE4" s="8"/>
-      <c r="AF4" s="9"/>
-      <c r="AG4" s="9"/>
-    </row>
-    <row r="5" spans="1:90" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="9"/>
+      <c r="AL4" s="9"/>
+    </row>
+    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>122</v>
       </c>
@@ -1610,114 +1673,138 @@
       <c r="I5" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="L5" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="M5" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="N5" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="O5" s="6"/>
-      <c r="P5" s="5" t="s">
+      <c r="Q5" s="6"/>
+      <c r="R5" s="26" t="s">
+        <v>225</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="T5" s="26" t="s">
+        <v>227</v>
+      </c>
+      <c r="U5" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="10"/>
-      <c r="AO5" s="9">
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="10"/>
+      <c r="AT5" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:90" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="6"/>
-      <c r="N6" s="6" t="s">
+      <c r="L6" s="6"/>
+      <c r="P6" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="O6" s="6"/>
-      <c r="P6" s="5" t="s">
+      <c r="Q6" s="6"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+    </row>
+    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="J7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="17"/>
+      <c r="L7" s="6"/>
       <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="17"/>
+      <c r="S7" s="17"/>
       <c r="T7" s="17"/>
       <c r="U7" s="6"/>
-      <c r="AL7" s="17" t="s">
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="17"/>
+      <c r="Z7" s="6"/>
+      <c r="AQ7" s="17" t="s">
         <v>159</v>
       </c>
-      <c r="AM7" s="5" t="s">
+      <c r="AR7" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AN7" s="17" t="s">
+      <c r="AS7" s="17" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="17" t="s">
+      <c r="P8" s="6"/>
+      <c r="Q8" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="AP8" s="5" t="s">
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="AU8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AQ8" s="5" t="s">
+      <c r="AV8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AR8" s="5">
+      <c r="AW8" s="5">
         <v>123456</v>
       </c>
-      <c r="AS8" s="5" t="s">
+      <c r="AX8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AT8" s="5" t="s">
+      <c r="AY8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AU8" s="5" t="s">
+      <c r="AZ8" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>142</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="AV9" s="5" t="s">
+      <c r="BA9" s="5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:90" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>143</v>
       </c>
@@ -1730,461 +1817,495 @@
       </c>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
-      <c r="M10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
       <c r="O10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
       <c r="T10" s="14"/>
-      <c r="AG10" s="14"/>
+      <c r="Y10" s="14"/>
       <c r="AL10" s="14"/>
-      <c r="AN10" s="14"/>
-      <c r="AW10" s="2" t="s">
+      <c r="AQ10" s="14"/>
+      <c r="AS10" s="14"/>
+      <c r="BB10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AX10" s="2" t="s">
+      <c r="BC10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AY10" s="2" t="s">
+      <c r="BD10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AZ10" s="2" t="s">
+      <c r="BE10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BA10" s="2" t="s">
+      <c r="BF10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BB10" s="2" t="s">
+      <c r="BG10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BC10" s="2">
+      <c r="BH10" s="2">
         <v>27</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="BI10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BE10" s="2" t="s">
+      <c r="BJ10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BF10" s="2" t="s">
+      <c r="BK10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BG10" s="2">
+      <c r="BL10" s="2">
         <v>2</v>
       </c>
-      <c r="BH10" s="2" t="s">
+      <c r="BM10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BI10" s="14"/>
-      <c r="BJ10" s="14"/>
-    </row>
-    <row r="11" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="BN10" s="14"/>
+      <c r="BO10" s="14"/>
+    </row>
+    <row r="11" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>144</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>160</v>
       </c>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
-    </row>
-    <row r="12" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="R11" s="17"/>
+      <c r="S11" s="17"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+    </row>
+    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>145</v>
       </c>
       <c r="G12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
-    </row>
-    <row r="13" spans="1:90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+    </row>
+    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>146</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="10"/>
-      <c r="AO13" s="9">
+      <c r="L13" s="6"/>
+      <c r="AN13" s="1"/>
+      <c r="AO13" s="10"/>
+      <c r="AT13" s="9">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>147</v>
       </c>
       <c r="H14" t="s">
         <v>129</v>
       </c>
-      <c r="BK14" s="5" t="s">
+      <c r="BP14" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>152</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="BL15" s="5" t="s">
+      <c r="BQ15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BM15" s="5" t="s">
+      <c r="BR15" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BN15" s="5" t="s">
+      <c r="BS15" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BO15" s="6" t="s">
+      <c r="BT15" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>161</v>
       </c>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
-      <c r="W16" s="20">
+      <c r="AB16" s="20">
         <v>3</v>
       </c>
-      <c r="BL16" s="5" t="s">
+      <c r="BQ16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="BM16" s="5" t="s">
+      <c r="BR16" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="BN16" s="6" t="s">
+      <c r="BS16" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>163</v>
       </c>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23"/>
-      <c r="W17" s="19" t="s">
+      <c r="AB17" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="BO17" s="5" t="s">
+      <c r="BT17" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:90" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="J18" s="6"/>
-      <c r="W18" s="5" t="s">
+      <c r="L18" s="6"/>
+      <c r="AB18" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="10"/>
-      <c r="AO18" s="9">
+      <c r="AN18" s="3"/>
+      <c r="AO18" s="10"/>
+      <c r="AT18" s="9">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A19" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
-      <c r="W19" s="5" t="s">
+      <c r="R19" s="17"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="AB19" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="AI19" s="1"/>
-    </row>
-    <row r="20" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AN19" s="1"/>
+    </row>
+    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A20" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="AE20" s="8"/>
-      <c r="AF20" s="9"/>
-      <c r="AG20" s="9"/>
-      <c r="AI20" s="11" t="s">
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="9"/>
+      <c r="AL20" s="9"/>
+      <c r="AN20" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="AJ20" s="21" t="s">
+      <c r="AO20" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="AO20" s="5">
+      <c r="AT20" s="5">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
       <c r="P21" s="6"/>
-      <c r="W21" s="15" t="s">
+      <c r="Q21" s="6"/>
+      <c r="R21" s="17"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="6"/>
+      <c r="AB21" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="X21" s="15" t="s">
+      <c r="AC21" s="15" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
       <c r="P22" s="6"/>
-      <c r="W22" s="15" t="s">
+      <c r="Q22" s="6"/>
+      <c r="R22" s="17"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="17"/>
+      <c r="U22" s="6"/>
+      <c r="AB22" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="AE22" s="11"/>
-    </row>
-    <row r="23" spans="1:90" x14ac:dyDescent="0.35">
+      <c r="AJ22" s="11"/>
+    </row>
+    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="K23" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="N23" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="Z23" s="5" t="s">
+      <c r="AE23" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="AA23" s="5" t="s">
+      <c r="AF23" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="AB23" s="15" t="s">
+      <c r="AG23" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="AC23" s="5" t="s">
+      <c r="AH23" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="AD23" s="15" t="s">
+      <c r="AI23" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="AE23" s="5">
+      <c r="AJ23" s="5">
         <v>33185</v>
       </c>
-      <c r="AF23" s="5">
+      <c r="AK23" s="5">
         <v>6546466555</v>
       </c>
     </row>
-    <row r="24" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="N24" s="6" t="s">
+      <c r="P24" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="O24" s="6"/>
-      <c r="P24" s="6"/>
-      <c r="W24" s="6"/>
-      <c r="Z24" s="23" t="s">
+      <c r="Q24" s="6"/>
+      <c r="R24" s="17"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="6"/>
+      <c r="AB24" s="6"/>
+      <c r="AE24" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="AA24" s="23" t="s">
+      <c r="AF24" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="AD24" s="23"/>
-      <c r="AE24" s="24"/>
-      <c r="AF24" s="24"/>
-      <c r="AH24" s="25"/>
-      <c r="BP24" s="5" t="s">
+      <c r="AI24" s="23"/>
+      <c r="AJ24" s="24"/>
+      <c r="AK24" s="24"/>
+      <c r="AM24" s="25"/>
+      <c r="BU24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="BQ24" s="5" t="s">
+      <c r="BV24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="BR24" s="5" t="s">
+      <c r="BW24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="BS24" s="5" t="s">
+      <c r="BX24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BT24" s="5" t="s">
+      <c r="BY24" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="BU24" s="5" t="s">
+      <c r="BZ24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="CA24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="BW24" s="5">
+      <c r="CB24" s="5">
         <v>9</v>
       </c>
-      <c r="BX24" s="5">
+      <c r="CC24" s="5">
         <v>10</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="CD24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="BZ24" s="12">
+      <c r="CE24" s="12">
         <v>40000</v>
       </c>
-      <c r="CA24" s="5">
+      <c r="CF24" s="5">
         <v>12</v>
       </c>
-      <c r="CB24" s="12">
+      <c r="CG24" s="12">
         <v>1000000</v>
       </c>
-      <c r="CC24" s="5" t="s">
+      <c r="CH24" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CI24" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="CE24" s="5">
+      <c r="CJ24" s="5">
         <v>57501</v>
       </c>
-      <c r="CF24" s="5" t="s">
+      <c r="CK24" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="CG24" s="5" t="s">
+      <c r="CL24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="CH24" s="5" t="s">
+      <c r="CM24" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="CI24" s="5" t="s">
+      <c r="CN24" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="CJ24" s="5" t="s">
+      <c r="CO24" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:90" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="J25" s="6"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
-      <c r="BI25" s="23" t="s">
+      <c r="R25" s="17"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="BN25" s="23" t="s">
         <v>197</v>
       </c>
-      <c r="BJ25" s="23" t="s">
+      <c r="BO25" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:90" ht="87" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:95" ht="87" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="K26" s="23" t="s">
+      <c r="M26" s="23" t="s">
         <v>200</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="N26" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="Z26" s="5" t="s">
+      <c r="AE26" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="AA26" s="5" t="s">
+      <c r="AF26" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="AD26" s="5" t="s">
+      <c r="AI26" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="AE26" s="11" t="s">
+      <c r="AJ26" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="AF26" s="11" t="s">
+      <c r="AK26" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="AH26" s="25" t="s">
+      <c r="AM26" s="25" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:90" ht="87" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:95" ht="87" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="K27" s="5" t="s">
+      <c r="M27" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="L27" s="5" t="s">
+      <c r="N27" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="N27" s="6"/>
-      <c r="O27" s="6"/>
       <c r="P27" s="6"/>
-      <c r="Z27" s="23" t="s">
+      <c r="Q27" s="6"/>
+      <c r="R27" s="17"/>
+      <c r="S27" s="17"/>
+      <c r="T27" s="17"/>
+      <c r="U27" s="6"/>
+      <c r="AE27" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="AA27" s="23" t="s">
+      <c r="AF27" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="AB27" s="23"/>
-      <c r="AC27" s="23"/>
-      <c r="AD27" s="23" t="s">
+      <c r="AG27" s="23"/>
+      <c r="AH27" s="23"/>
+      <c r="AI27" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="AE27" s="23">
+      <c r="AJ27" s="23">
         <v>19801</v>
       </c>
-      <c r="AF27" s="23">
+      <c r="AK27" s="23">
         <v>9898989898</v>
       </c>
-      <c r="AG27" s="23"/>
-      <c r="AH27" s="25" t="s">
+      <c r="AL27" s="23"/>
+      <c r="AM27" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="AI27" s="25"/>
-    </row>
-    <row r="30" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="CK30" s="5" t="s">
+      <c r="AN27" s="25"/>
+    </row>
+    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
+      <c r="CP30" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="CK31" s="5" t="s">
+    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
+      <c r="CP31" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:90" x14ac:dyDescent="0.35">
-      <c r="CL32" s="5" t="s">
+    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
+      <c r="CQ32" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="10:16" x14ac:dyDescent="0.35">
-      <c r="J33" s="6"/>
-      <c r="N33" s="6"/>
-      <c r="O33" s="6"/>
+    <row r="33" spans="12:21" x14ac:dyDescent="0.35">
+      <c r="L33" s="6"/>
       <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="BO15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BT15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
-    <hyperlink ref="N6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
-    <hyperlink ref="N5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
+    <hyperlink ref="P6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
+    <hyperlink ref="L4" r:id="rId5" xr:uid="{F5509D6D-69DD-4627-8344-90D45126A4BD}"/>
     <hyperlink ref="E4" r:id="rId6" xr:uid="{547248F2-378C-415E-95A7-678C1DBD77A8}"/>
-    <hyperlink ref="N2" r:id="rId7" xr:uid="{A3F582FF-4788-4DAE-ABAC-5439277BD83D}"/>
-    <hyperlink ref="M2" r:id="rId8" xr:uid="{09DDF643-6769-411C-9C0A-0F3FFD7CCB83}"/>
+    <hyperlink ref="P2" r:id="rId7" xr:uid="{A3F582FF-4788-4DAE-ABAC-5439277BD83D}"/>
+    <hyperlink ref="O2" r:id="rId8" xr:uid="{09DDF643-6769-411C-9C0A-0F3FFD7CCB83}"/>
     <hyperlink ref="I2" r:id="rId9" xr:uid="{79A5204C-1E5E-4D7D-BE23-3D875D65F089}"/>
-    <hyperlink ref="AL7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
-    <hyperlink ref="J2" r:id="rId11" xr:uid="{6BA18CB7-8C64-4E80-8B31-7A3FF7879487}"/>
+    <hyperlink ref="AQ7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
+    <hyperlink ref="L2" r:id="rId11" xr:uid="{6BA18CB7-8C64-4E80-8B31-7A3FF7879487}"/>
     <hyperlink ref="B2" r:id="rId12" xr:uid="{0899709A-6969-4E02-AE8C-00614240DAC5}"/>
     <hyperlink ref="D2" r:id="rId13" xr:uid="{1B2A8791-D86B-44BD-9CED-0E6631F993F1}"/>
+    <hyperlink ref="J5" r:id="rId14" xr:uid="{0D38F4D9-15FF-4CC9-ADA8-CA20963E5762}"/>
+    <hyperlink ref="K5" r:id="rId15" xr:uid="{D74E6246-268E-42AF-A63A-269863ADC9EA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId14"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
OXO-We are here for you section-Testcase,helper,testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7F4C23-FCEF-4B42-8853-924BBEFC1435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B0B3D3-AF34-4D12-AC82-2D6AB03CB86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="235">
   <si>
     <t>UserName</t>
   </si>
@@ -720,6 +720,27 @@
   <si>
     <t>The password doesn't match this account. Verify the password and try again.</t>
   </si>
+  <si>
+    <t>SuccessPage</t>
+  </si>
+  <si>
+    <t>Chat live with our service reps,Call our service line. Reach out to us at,Drop us a message to our customer support box</t>
+  </si>
+  <si>
+    <t>tel:1234567890,mailto:support@hydroflask.com</t>
+  </si>
+  <si>
+    <t>Kitchenware,coffee-beverage</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>hyperlink</t>
+  </si>
+  <si>
+    <t>categorylinks</t>
+  </si>
 </sst>
 </file>
 
@@ -728,7 +749,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -764,8 +785,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -776,6 +812,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -792,7 +834,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -803,35 +845,33 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1113,115 +1153,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CQ33"/>
+  <dimension ref="A1:CT33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.7265625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="30.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.7265625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="80.81640625" style="15" customWidth="1"/>
-    <col min="9" max="11" width="30.7265625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.1796875" style="15" customWidth="1"/>
-    <col min="16" max="16" width="30.7265625" style="5" customWidth="1"/>
-    <col min="17" max="17" width="54.81640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="54.81640625" style="15" customWidth="1"/>
-    <col min="21" max="21" width="96.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="61.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="23.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.54296875" style="15" customWidth="1"/>
-    <col min="26" max="26" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="9.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="30.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.1796875" style="5" customWidth="1"/>
-    <col min="32" max="32" width="20.54296875" style="5" customWidth="1"/>
-    <col min="33" max="33" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11" style="15" customWidth="1"/>
-    <col min="39" max="39" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="36.26953125" style="15" customWidth="1"/>
-    <col min="44" max="44" width="56.81640625" style="5"/>
-    <col min="45" max="45" width="56.81640625" style="15"/>
-    <col min="46" max="46" width="5.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="11.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="11.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="29.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="15.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="161.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="9.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="10.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="4.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="7.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="20.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="23.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="35.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="35.453125" style="15" customWidth="1"/>
-    <col min="68" max="68" width="146.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="16.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="15" style="5" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="28.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="43.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="21.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="6.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="12.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="13.1796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="6.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="15.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="7.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="17.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="15.54296875" style="5" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="6.26953125" style="5" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="11.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="7.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="14" style="5" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="5" style="5" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="18.81640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="94" max="94" width="255.7265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="10.453125" style="5" bestFit="1" customWidth="1"/>
-    <col min="96" max="16384" width="56.81640625" style="5"/>
+    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.77734375" customWidth="1"/>
+    <col min="5" max="5" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="80.77734375" customWidth="1"/>
+    <col min="9" max="11" width="30.77734375" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.21875" customWidth="1"/>
+    <col min="16" max="16" width="30.77734375" customWidth="1"/>
+    <col min="17" max="17" width="54.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="54.77734375" customWidth="1"/>
+    <col min="24" max="24" width="96.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="61.5546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.5546875" customWidth="1"/>
+    <col min="29" max="29" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.21875" customWidth="1"/>
+    <col min="35" max="35" width="20.5546875" customWidth="1"/>
+    <col min="36" max="36" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11" customWidth="1"/>
+    <col min="42" max="42" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="10" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="36.21875" customWidth="1"/>
+    <col min="49" max="49" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="161.44140625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="35.44140625" customWidth="1"/>
+    <col min="71" max="71" width="146.77734375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="43.5546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="12" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="17" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="8" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="14" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="255.77734375" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="4" t="s">
         <v>210</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -1239,10 +1276,10 @@
       <c r="I1" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="J1" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="4" t="s">
         <v>220</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -1260,1036 +1297,1177 @@
       <c r="P1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="Q1" s="16" t="s">
+      <c r="Q1" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="R1" s="22" t="s">
+      <c r="R1" s="4" t="s">
         <v>222</v>
       </c>
       <c r="S1" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="T1" s="22" t="s">
+        <v>233</v>
+      </c>
+      <c r="U1" s="22" t="s">
+        <v>234</v>
+      </c>
+      <c r="V1" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="W1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AC1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AP1" s="4" t="s">
+      <c r="AS1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AT1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="AR1" s="4" t="s">
+      <c r="AU1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="AS1" s="4" t="s">
+      <c r="AV1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AT1" s="4" t="s">
+      <c r="AW1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AU1" s="5" t="s">
+      <c r="AX1" t="s">
         <v>23</v>
       </c>
-      <c r="AV1" s="4" t="s">
+      <c r="AY1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AW1" s="4" t="s">
+      <c r="AZ1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AX1" s="4" t="s">
+      <c r="BA1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AY1" s="4" t="s">
+      <c r="BB1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AZ1" s="4" t="s">
+      <c r="BC1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="BA1" s="4" t="s">
+      <c r="BD1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="BB1" s="4" t="s">
+      <c r="BE1" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="BC1" s="4" t="s">
+      <c r="BF1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="BD1" s="4" t="s">
+      <c r="BG1" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="BE1" s="4" t="s">
+      <c r="BH1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="BF1" s="4" t="s">
+      <c r="BI1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="BG1" s="4" t="s">
+      <c r="BJ1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="BH1" s="4" t="s">
+      <c r="BK1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="BI1" s="4" t="s">
+      <c r="BL1" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="BJ1" s="4" t="s">
+      <c r="BM1" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BK1" s="4" t="s">
+      <c r="BN1" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BL1" s="4" t="s">
+      <c r="BO1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="BM1" s="4" t="s">
+      <c r="BP1" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="BN1" s="22" t="s">
+      <c r="BQ1" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="BO1" s="22" t="s">
+      <c r="BR1" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="BP1" s="4" t="s">
+      <c r="BS1" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="BQ1" s="4" t="s">
+      <c r="BT1" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="BR1" s="4" t="s">
+      <c r="BU1" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="BS1" s="4" t="s">
+      <c r="BV1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="BT1" s="4" t="s">
+      <c r="BW1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="BU1" s="4" t="s">
+      <c r="BX1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BV1" s="4" t="s">
+      <c r="BY1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="BW1" s="4" t="s">
+      <c r="BZ1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="BX1" s="4" t="s">
+      <c r="CA1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="BY1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="BZ1" s="4" t="s">
+      <c r="CC1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CD1" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="CB1" s="4" t="s">
+      <c r="CE1" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="CC1" s="4" t="s">
+      <c r="CF1" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="CD1" s="4" t="s">
+      <c r="CG1" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CH1" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="CF1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="CG1" s="4" t="s">
+      <c r="CJ1" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CK1" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="CI1" s="4" t="s">
+      <c r="CL1" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="CJ1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="CK1" s="4" t="s">
+      <c r="CN1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="CL1" s="4" t="s">
+      <c r="CO1" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="CM1" s="4" t="s">
+      <c r="CP1" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="CN1" s="4" t="s">
+      <c r="CQ1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="CO1" s="4" t="s">
+      <c r="CR1" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="CP1" s="5" t="s">
+      <c r="CS1" t="s">
         <v>103</v>
       </c>
-      <c r="CQ1" s="5" t="s">
+      <c r="CT1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" t="s">
         <v>212</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" t="s">
         <v>130</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" t="s">
         <v>131</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="17" t="s">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AC2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AD2" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="AB2" s="6"/>
-      <c r="AC2" s="6"/>
-      <c r="AD2" s="6"/>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" t="s">
         <v>133</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AI2" t="s">
         <v>134</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AJ2" t="s">
         <v>177</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AK2" t="s">
         <v>169</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AL2" t="s">
         <v>169</v>
       </c>
-      <c r="AJ2" s="11" t="s">
+      <c r="AM2" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="AK2" s="5">
+      <c r="AN2">
         <v>9898989898</v>
       </c>
-      <c r="AL2" s="15" t="s">
+      <c r="AO2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>110</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" t="s">
         <v>113</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="15" t="s">
+      <c r="L3" s="5"/>
+      <c r="M3" t="s">
         <v>130</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" t="s">
         <v>131</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
-      <c r="T3" s="17"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="7" t="s">
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="17"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AJ3" s="8"/>
-      <c r="AK3" s="9"/>
-      <c r="AL3" s="9"/>
-    </row>
-    <row r="4" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AM3" s="7"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+    </row>
+    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>115</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="6" t="s">
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" t="s">
         <v>130</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" t="s">
         <v>131</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
-      <c r="T4" s="17"/>
-      <c r="U4" s="5" t="s">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" t="s">
         <v>117</v>
       </c>
-      <c r="V4" s="7"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="17"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="6"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-    </row>
-    <row r="5" spans="1:95" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AM4" s="7"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+    </row>
+    <row r="5" spans="1:98" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>122</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17" t="s">
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
         <v>191</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="K5" s="17" t="s">
+      <c r="K5" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" t="s">
         <v>130</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P5" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="26" t="s">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="S5" s="7" t="s">
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="T5" s="26" t="s">
+      <c r="W5" s="16" t="s">
         <v>227</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="X5" t="s">
         <v>120</v>
       </c>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="10"/>
-      <c r="AT5" s="9">
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="9"/>
+      <c r="AW5" s="8">
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:95" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>123</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="P6" s="6" t="s">
+      <c r="L6" s="5"/>
+      <c r="P6" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="5" t="s">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="W6" s="5"/>
+      <c r="X6" t="s">
         <v>120</v>
       </c>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="6"/>
-    </row>
-    <row r="7" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A7" s="5" t="s">
+      <c r="Y6" s="5"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="5"/>
+      <c r="AB6" s="5"/>
+      <c r="AC6" s="5"/>
+      <c r="AD6" s="5"/>
+      <c r="AE6" s="5"/>
+      <c r="AF6" s="5"/>
+      <c r="AG6" s="5"/>
+    </row>
+    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>125</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="17"/>
-      <c r="Z7" s="6"/>
-      <c r="AQ7" s="17" t="s">
+      <c r="L7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="5"/>
+      <c r="X7" s="5"/>
+      <c r="Y7" s="5"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="5"/>
+      <c r="AB7" s="5"/>
+      <c r="AC7" s="5"/>
+      <c r="AT7" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="AR7" s="5" t="s">
+      <c r="AU7" t="s">
         <v>126</v>
       </c>
-      <c r="AS7" s="17" t="s">
+      <c r="AV7" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>127</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="17" t="s">
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="6"/>
-      <c r="V8" s="6"/>
-      <c r="AU8" s="5" t="s">
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="AX8" t="s">
         <v>24</v>
       </c>
-      <c r="AV8" s="5" t="s">
+      <c r="AY8" t="s">
         <v>26</v>
       </c>
-      <c r="AW8" s="5">
+      <c r="AZ8">
         <v>123456</v>
       </c>
-      <c r="AX8" s="5" t="s">
+      <c r="BA8" t="s">
         <v>29</v>
       </c>
-      <c r="AY8" s="5" t="s">
+      <c r="BB8" t="s">
         <v>31</v>
       </c>
-      <c r="AZ8" s="5" t="s">
+      <c r="BC8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>142</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" t="s">
         <v>148</v>
       </c>
-      <c r="BA9" s="5" t="s">
+      <c r="BD9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:95" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AQ10" s="14"/>
-      <c r="AS10" s="14"/>
-      <c r="BB10" s="2" t="s">
+      <c r="BE10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="BC10" s="2" t="s">
+      <c r="BF10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="BD10" s="2" t="s">
+      <c r="BG10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="BE10" s="2" t="s">
+      <c r="BH10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="BF10" s="2" t="s">
+      <c r="BI10" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="BG10" s="2" t="s">
+      <c r="BJ10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="BH10" s="2">
+      <c r="BK10" s="2">
         <v>27</v>
       </c>
-      <c r="BI10" s="2" t="s">
+      <c r="BL10" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="BJ10" s="2" t="s">
+      <c r="BM10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="BK10" s="2" t="s">
+      <c r="BN10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="BL10" s="2">
+      <c r="BO10" s="2">
         <v>2</v>
       </c>
-      <c r="BM10" s="2" t="s">
+      <c r="BP10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="BN10" s="14"/>
-      <c r="BO10" s="14"/>
-    </row>
-    <row r="11" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
+    </row>
+    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>144</v>
       </c>
-      <c r="G11" s="15" t="s">
+      <c r="G11" t="s">
         <v>160</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="17"/>
-      <c r="S11" s="17"/>
-      <c r="T11" s="17"/>
-      <c r="U11" s="6"/>
-      <c r="V11" s="6"/>
-    </row>
-    <row r="12" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+      <c r="W11" s="5"/>
+      <c r="X11" s="5"/>
+      <c r="Y11" s="5"/>
+    </row>
+    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>145</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" t="s">
         <v>150</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="17"/>
-      <c r="U12" s="6"/>
-      <c r="V12" s="6"/>
-    </row>
-    <row r="13" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="P12" s="5"/>
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+      <c r="W12" s="5"/>
+      <c r="X12" s="5"/>
+      <c r="Y12" s="5"/>
+    </row>
+    <row r="13" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="15" t="s">
+      <c r="G13" t="s">
         <v>151</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="AN13" s="1"/>
-      <c r="AO13" s="10"/>
-      <c r="AT13" s="9">
+      <c r="L13" s="5"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="9"/>
+      <c r="AW13" s="8">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>147</v>
       </c>
       <c r="H14" t="s">
         <v>129</v>
       </c>
-      <c r="BP14" s="5" t="s">
+      <c r="BS14" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>152</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" t="s">
         <v>154</v>
       </c>
-      <c r="BQ15" s="5" t="s">
+      <c r="BT15" t="s">
         <v>105</v>
       </c>
-      <c r="BR15" s="5" t="s">
+      <c r="BU15" t="s">
         <v>106</v>
       </c>
-      <c r="BS15" s="5" t="s">
+      <c r="BV15" t="s">
         <v>107</v>
       </c>
-      <c r="BT15" s="6" t="s">
+      <c r="BW15" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A16" s="18" t="s">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="AB16" s="20">
+      <c r="AE16" s="13">
         <v>3</v>
       </c>
-      <c r="BQ16" s="5" t="s">
+      <c r="BT16" t="s">
         <v>108</v>
       </c>
-      <c r="BR16" s="5" t="s">
+      <c r="BU16" t="s">
         <v>109</v>
       </c>
-      <c r="BS16" s="6" t="s">
+      <c r="BV16" s="5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>163</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="AB17" s="19" t="s">
+      <c r="AE17" t="s">
         <v>162</v>
       </c>
-      <c r="BT17" s="5" t="s">
+      <c r="BW17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:95" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>165</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="AB18" s="5" t="s">
+      <c r="L18" s="5"/>
+      <c r="AE18" t="s">
         <v>166</v>
       </c>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="10"/>
-      <c r="AT18" s="9">
+      <c r="AQ18" s="3"/>
+      <c r="AR18" s="9"/>
+      <c r="AW18" s="8">
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>168</v>
       </c>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="17"/>
-      <c r="S19" s="17"/>
-      <c r="T19" s="17"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="AB19" s="5" t="s">
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="AE19" t="s">
         <v>174</v>
       </c>
-      <c r="AN19" s="1"/>
-    </row>
-    <row r="20" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
+      <c r="AQ19" s="1"/>
+    </row>
+    <row r="20" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
         <v>170</v>
       </c>
-      <c r="AJ20" s="8"/>
-      <c r="AK20" s="9"/>
-      <c r="AL20" s="9"/>
-      <c r="AN20" s="11" t="s">
+      <c r="AM20" s="7"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AQ20" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="AO20" s="21" t="s">
+      <c r="AR20" s="14" t="s">
         <v>173</v>
       </c>
-      <c r="AT20" s="5">
+      <c r="AW20">
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A21" s="15" t="s">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>180</v>
       </c>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="17"/>
-      <c r="S21" s="17"/>
-      <c r="T21" s="17"/>
-      <c r="U21" s="6"/>
-      <c r="AB21" s="15" t="s">
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="AE21" t="s">
         <v>178</v>
       </c>
-      <c r="AC21" s="15" t="s">
+      <c r="AF21" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>181</v>
       </c>
-      <c r="P22" s="6"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="17"/>
-      <c r="S22" s="17"/>
-      <c r="T22" s="17"/>
-      <c r="U22" s="6"/>
-      <c r="AB22" s="15" t="s">
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="AE22" t="s">
         <v>182</v>
       </c>
-      <c r="AJ22" s="11"/>
-    </row>
-    <row r="23" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
+      <c r="AM22" s="10"/>
+    </row>
+    <row r="23" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>183</v>
       </c>
-      <c r="M23" s="5" t="s">
+      <c r="M23" t="s">
         <v>184</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" t="s">
         <v>185</v>
       </c>
-      <c r="AE23" s="5" t="s">
+      <c r="AH23" t="s">
         <v>186</v>
       </c>
-      <c r="AF23" s="5" t="s">
+      <c r="AI23" t="s">
         <v>187</v>
       </c>
-      <c r="AG23" s="15" t="s">
+      <c r="AJ23" t="s">
         <v>189</v>
       </c>
-      <c r="AH23" s="5" t="s">
+      <c r="AK23" t="s">
         <v>188</v>
       </c>
-      <c r="AI23" s="15" t="s">
+      <c r="AL23" t="s">
         <v>188</v>
       </c>
-      <c r="AJ23" s="5">
+      <c r="AM23">
         <v>33185</v>
       </c>
-      <c r="AK23" s="5">
+      <c r="AN23">
         <v>6546466555</v>
       </c>
     </row>
-    <row r="24" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>192</v>
       </c>
-      <c r="P24" s="6" t="s">
+      <c r="P24" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="17"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="17"/>
-      <c r="U24" s="6"/>
-      <c r="AB24" s="6"/>
-      <c r="AE24" s="23" t="s">
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="5"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="5"/>
+      <c r="V24" s="5"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AH24" t="s">
         <v>201</v>
       </c>
-      <c r="AF24" s="23" t="s">
+      <c r="AI24" t="s">
         <v>202</v>
       </c>
-      <c r="AI24" s="23"/>
-      <c r="AJ24" s="24"/>
-      <c r="AK24" s="24"/>
-      <c r="AM24" s="25"/>
-      <c r="BU24" s="5" t="s">
+      <c r="AM24" s="10"/>
+      <c r="AN24" s="10"/>
+      <c r="AP24" s="15"/>
+      <c r="BX24" t="s">
         <v>69</v>
       </c>
-      <c r="BV24" s="5" t="s">
+      <c r="BY24" t="s">
         <v>70</v>
       </c>
-      <c r="BW24" s="5" t="s">
+      <c r="BZ24" t="s">
         <v>71</v>
       </c>
-      <c r="BX24" s="5" t="s">
+      <c r="CA24" t="s">
         <v>43</v>
       </c>
-      <c r="BY24" s="5" t="s">
+      <c r="CB24" t="s">
         <v>43</v>
       </c>
-      <c r="BZ24" s="5" t="s">
+      <c r="CC24" t="s">
         <v>72</v>
       </c>
-      <c r="CA24" s="5" t="s">
+      <c r="CD24" t="s">
         <v>72</v>
       </c>
-      <c r="CB24" s="5">
+      <c r="CE24">
         <v>9</v>
       </c>
-      <c r="CC24" s="5">
+      <c r="CF24">
         <v>10</v>
       </c>
-      <c r="CD24" s="5" t="s">
+      <c r="CG24" t="s">
         <v>73</v>
       </c>
-      <c r="CE24" s="12">
+      <c r="CH24" s="11">
         <v>40000</v>
       </c>
-      <c r="CF24" s="5">
+      <c r="CI24">
         <v>12</v>
       </c>
-      <c r="CG24" s="12">
+      <c r="CJ24" s="11">
         <v>1000000</v>
       </c>
-      <c r="CH24" s="5" t="s">
+      <c r="CK24" t="s">
         <v>34</v>
       </c>
-      <c r="CI24" s="5" t="s">
+      <c r="CL24" t="s">
         <v>74</v>
       </c>
-      <c r="CJ24" s="5">
+      <c r="CM24">
         <v>57501</v>
       </c>
-      <c r="CK24" s="5" t="s">
+      <c r="CN24" t="s">
         <v>75</v>
       </c>
-      <c r="CL24" s="5" t="s">
+      <c r="CO24" t="s">
         <v>76</v>
       </c>
-      <c r="CM24" s="5" t="s">
+      <c r="CP24" t="s">
         <v>77</v>
       </c>
-      <c r="CN24" s="5" t="s">
+      <c r="CQ24" t="s">
         <v>71</v>
       </c>
-      <c r="CO24" s="5" t="s">
+      <c r="CR24" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
+    <row r="25" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>194</v>
       </c>
-      <c r="L25" s="6"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="6"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="17"/>
-      <c r="S25" s="17"/>
-      <c r="T25" s="17"/>
-      <c r="U25" s="6"/>
-      <c r="V25" s="6"/>
-      <c r="BN25" s="23" t="s">
+      <c r="L25" s="5"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+      <c r="S25" s="5"/>
+      <c r="T25" s="5"/>
+      <c r="U25" s="5"/>
+      <c r="V25" s="5"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="BQ25" t="s">
         <v>197</v>
       </c>
-      <c r="BO25" s="23" t="s">
+      <c r="BR25" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:95" ht="87" x14ac:dyDescent="0.35">
-      <c r="A26" s="15" t="s">
+    <row r="26" spans="1:98" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>199</v>
       </c>
-      <c r="M26" s="23" t="s">
+      <c r="M26" t="s">
         <v>200</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N26" t="s">
         <v>130</v>
       </c>
-      <c r="AE26" s="5" t="s">
+      <c r="AH26" t="s">
         <v>201</v>
       </c>
-      <c r="AF26" s="5" t="s">
+      <c r="AI26" t="s">
         <v>202</v>
       </c>
-      <c r="AI26" s="5" t="s">
+      <c r="AL26" t="s">
         <v>203</v>
       </c>
-      <c r="AJ26" s="11" t="s">
+      <c r="AM26" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="AK26" s="11" t="s">
+      <c r="AN26" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="AM26" s="25" t="s">
+      <c r="AP26" s="15" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:95" ht="87" x14ac:dyDescent="0.35">
-      <c r="A27" s="15" t="s">
+    <row r="27" spans="1:98" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>214</v>
       </c>
-      <c r="M27" s="5" t="s">
+      <c r="M27" t="s">
         <v>131</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" t="s">
         <v>131</v>
       </c>
-      <c r="P27" s="6"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="17"/>
-      <c r="S27" s="17"/>
-      <c r="T27" s="17"/>
-      <c r="U27" s="6"/>
-      <c r="AE27" s="23" t="s">
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="AH27" t="s">
         <v>215</v>
       </c>
-      <c r="AF27" s="23" t="s">
+      <c r="AI27" t="s">
         <v>216</v>
       </c>
-      <c r="AG27" s="23"/>
-      <c r="AH27" s="23"/>
-      <c r="AI27" s="23" t="s">
+      <c r="AL27" t="s">
         <v>217</v>
       </c>
-      <c r="AJ27" s="23">
+      <c r="AM27">
         <v>19801</v>
       </c>
-      <c r="AK27" s="23">
+      <c r="AN27">
         <v>9898989898</v>
       </c>
-      <c r="AL27" s="23"/>
-      <c r="AM27" s="25" t="s">
+      <c r="AP27" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="AN27" s="25"/>
-    </row>
-    <row r="30" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="CP30" s="5" t="s">
+      <c r="AQ27" s="15"/>
+    </row>
+    <row r="28" spans="1:98" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="20"/>
+      <c r="S28" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="T28" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="U28" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="V28" s="18"/>
+      <c r="W28" s="19"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="20"/>
+      <c r="Z28" s="20"/>
+      <c r="AA28" s="20"/>
+      <c r="AB28" s="20"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="18"/>
+      <c r="AE28" s="19"/>
+      <c r="AF28" s="17"/>
+      <c r="AG28" s="17"/>
+      <c r="AH28" s="17"/>
+      <c r="AI28" s="17"/>
+      <c r="AJ28" s="17"/>
+      <c r="AK28" s="17"/>
+      <c r="AL28" s="17"/>
+      <c r="AM28" s="17"/>
+      <c r="AN28" s="17"/>
+      <c r="AO28" s="17"/>
+      <c r="AP28" s="17"/>
+      <c r="AQ28" s="17"/>
+      <c r="AR28" s="17"/>
+      <c r="AS28" s="17"/>
+      <c r="AT28" s="17"/>
+      <c r="AU28" s="17"/>
+      <c r="AV28" s="17"/>
+      <c r="AW28" s="17"/>
+      <c r="AX28" s="17"/>
+      <c r="AY28" s="17"/>
+      <c r="AZ28" s="17"/>
+      <c r="BA28" s="17"/>
+      <c r="BB28" s="21"/>
+      <c r="BC28" s="21"/>
+      <c r="BD28" s="17"/>
+      <c r="BE28" s="17"/>
+      <c r="BF28" s="17"/>
+      <c r="BG28" s="17"/>
+      <c r="BH28" s="17"/>
+      <c r="BI28" s="17"/>
+      <c r="BJ28" s="17"/>
+      <c r="BK28" s="17"/>
+      <c r="BL28" s="17"/>
+      <c r="BM28" s="17"/>
+      <c r="BN28" s="17"/>
+      <c r="BO28" s="17"/>
+      <c r="BP28" s="17"/>
+      <c r="BQ28" s="17"/>
+      <c r="BR28" s="21"/>
+      <c r="BS28" s="21"/>
+      <c r="BT28" s="17"/>
+      <c r="BU28" s="17"/>
+      <c r="BV28" s="17"/>
+      <c r="BW28" s="17"/>
+      <c r="BX28" s="17"/>
+      <c r="BY28" s="17"/>
+      <c r="BZ28" s="17"/>
+      <c r="CA28" s="17"/>
+      <c r="CB28" s="17"/>
+      <c r="CC28" s="17"/>
+      <c r="CD28" s="17"/>
+      <c r="CE28" s="17"/>
+      <c r="CF28" s="17"/>
+      <c r="CG28" s="21"/>
+      <c r="CH28" s="21"/>
+      <c r="CI28" s="17"/>
+      <c r="CJ28" s="21"/>
+      <c r="CK28" s="21"/>
+      <c r="CL28" s="17"/>
+      <c r="CM28" s="17"/>
+      <c r="CN28" s="17"/>
+      <c r="CO28" s="17"/>
+      <c r="CP28" s="17"/>
+      <c r="CQ28" s="21"/>
+      <c r="CR28" s="21"/>
+    </row>
+    <row r="30" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="CS30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="CP31" s="5" t="s">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="CS31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:95" x14ac:dyDescent="0.35">
-      <c r="CQ32" s="5" t="s">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="CT32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="12:21" x14ac:dyDescent="0.35">
-      <c r="L33" s="6"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="17"/>
-      <c r="S33" s="17"/>
-      <c r="T33" s="17"/>
-      <c r="U33" s="6"/>
+    <row r="33" spans="12:24" x14ac:dyDescent="0.3">
+      <c r="L33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="BB28:BC28"/>
+    <mergeCell ref="BR28:BS28"/>
+    <mergeCell ref="CG28:CH28"/>
+    <mergeCell ref="CJ28:CK28"/>
+    <mergeCell ref="CQ28:CR28"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="BT15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="BW15" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{70516023-68E4-47F0-944B-0FBC3753CCA5}"/>
     <hyperlink ref="P6" r:id="rId3" xr:uid="{1E011C06-6519-4126-9359-44AC1937A692}"/>
     <hyperlink ref="P5" r:id="rId4" xr:uid="{D4F9BB60-04BF-4801-AC3B-6A79C3F1D606}"/>
@@ -2298,14 +2476,15 @@
     <hyperlink ref="P2" r:id="rId7" xr:uid="{A3F582FF-4788-4DAE-ABAC-5439277BD83D}"/>
     <hyperlink ref="O2" r:id="rId8" xr:uid="{09DDF643-6769-411C-9C0A-0F3FFD7CCB83}"/>
     <hyperlink ref="I2" r:id="rId9" xr:uid="{79A5204C-1E5E-4D7D-BE23-3D875D65F089}"/>
-    <hyperlink ref="AQ7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
+    <hyperlink ref="AT7" r:id="rId10" xr:uid="{9B458FA4-6794-4C31-8CE4-8BD232D484A9}"/>
     <hyperlink ref="L2" r:id="rId11" xr:uid="{6BA18CB7-8C64-4E80-8B31-7A3FF7879487}"/>
     <hyperlink ref="B2" r:id="rId12" xr:uid="{0899709A-6969-4E02-AE8C-00614240DAC5}"/>
     <hyperlink ref="D2" r:id="rId13" xr:uid="{1B2A8791-D86B-44BD-9CED-0E6631F993F1}"/>
     <hyperlink ref="J5" r:id="rId14" xr:uid="{0D38F4D9-15FF-4CC9-ADA8-CA20963E5762}"/>
     <hyperlink ref="K5" r:id="rId15" xr:uid="{D74E6246-268E-42AF-A63A-269863ADC9EA}"/>
+    <hyperlink ref="T28" r:id="rId16" xr:uid="{4D45DB4D-31F8-41D6-BE3D-6D14DAE2B1DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Oxo, Hydro, helper, unit testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/OxoTestData.xlsx
+++ b/src/test/resources/TestData/OXO/OxoTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B0B3D3-AF34-4D12-AC82-2D6AB03CB86B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96326A3-5F05-4FA1-AABD-1E77548E61EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20391" windowHeight="11078" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="238">
   <si>
     <t>UserName</t>
   </si>
@@ -740,6 +740,15 @@
   </si>
   <si>
     <t>categorylinks</t>
+  </si>
+  <si>
+    <t>invalidPaymentDetails</t>
+  </si>
+  <si>
+    <t>424242424242424</t>
+  </si>
+  <si>
+    <t>04/20</t>
   </si>
 </sst>
 </file>
@@ -834,7 +843,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -870,8 +879,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1155,100 +1166,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CT33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="AI31" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.81640625" defaultRowHeight="14.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.77734375" customWidth="1"/>
-    <col min="8" max="8" width="80.77734375" customWidth="1"/>
-    <col min="9" max="11" width="30.77734375" customWidth="1"/>
-    <col min="12" max="12" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.21875" customWidth="1"/>
-    <col min="16" max="16" width="30.77734375" customWidth="1"/>
-    <col min="17" max="17" width="54.77734375" bestFit="1" customWidth="1"/>
-    <col min="18" max="23" width="54.77734375" customWidth="1"/>
-    <col min="24" max="24" width="96.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="61.5546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="23.77734375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.5546875" customWidth="1"/>
-    <col min="29" max="29" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.81640625" customWidth="1"/>
+    <col min="8" max="8" width="80.81640625" customWidth="1"/>
+    <col min="9" max="11" width="30.81640625" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.1796875" customWidth="1"/>
+    <col min="16" max="16" width="30.81640625" customWidth="1"/>
+    <col min="17" max="17" width="54.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="23" width="54.81640625" customWidth="1"/>
+    <col min="24" max="24" width="96.81640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="61.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.54296875" customWidth="1"/>
+    <col min="29" max="29" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.81640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="19" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="24.21875" customWidth="1"/>
-    <col min="35" max="35" width="20.5546875" customWidth="1"/>
-    <col min="36" max="36" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="24.1796875" customWidth="1"/>
+    <col min="35" max="35" width="20.54296875" customWidth="1"/>
+    <col min="36" max="36" width="11.54296875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="11" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9.1796875" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="11" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11" customWidth="1"/>
-    <col min="42" max="42" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.1796875" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="8" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="10" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="36.21875" customWidth="1"/>
-    <col min="49" max="49" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="161.44140625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="23.21875" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="35.44140625" customWidth="1"/>
-    <col min="71" max="71" width="146.77734375" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="36.1796875" customWidth="1"/>
+    <col min="49" max="49" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="161.453125" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="35.453125" customWidth="1"/>
+    <col min="71" max="71" width="146.81640625" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.81640625" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="28.77734375" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="12" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="6.1796875" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="15.453125" bestFit="1" customWidth="1"/>
     <col min="85" max="85" width="17" bestFit="1" customWidth="1"/>
-    <col min="86" max="86" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="7.81640625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="17.81640625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="6.1796875" bestFit="1" customWidth="1"/>
     <col min="91" max="91" width="8" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="93" max="93" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="93" max="93" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="14" bestFit="1" customWidth="1"/>
     <col min="95" max="95" width="5" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="255.77734375" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="255.81640625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -1303,13 +1314,13 @@
       <c r="R1" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="S1" s="22" t="s">
+      <c r="S1" s="21" t="s">
         <v>232</v>
       </c>
-      <c r="T1" s="22" t="s">
+      <c r="T1" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="U1" s="22" t="s">
+      <c r="U1" s="21" t="s">
         <v>234</v>
       </c>
       <c r="V1" s="4" t="s">
@@ -1544,7 +1555,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1629,7 +1640,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -1667,7 +1678,7 @@
       <c r="AN3" s="8"/>
       <c r="AO3" s="8"/>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>115</v>
       </c>
@@ -1715,7 +1726,7 @@
       <c r="AN4" s="8"/>
       <c r="AO4" s="8"/>
     </row>
-    <row r="5" spans="1:98" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:98" ht="24.7" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>122</v>
       </c>
@@ -1768,7 +1779,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:98" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:98" ht="13.55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -1796,7 +1807,7 @@
       <c r="AF6" s="5"/>
       <c r="AG6" s="5"/>
     </row>
-    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1860,7 +1871,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>142</v>
       </c>
@@ -1871,7 +1882,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:98" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>143</v>
       </c>
@@ -1915,7 +1926,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>144</v>
       </c>
@@ -1933,7 +1944,7 @@
       <c r="X11" s="5"/>
       <c r="Y11" s="5"/>
     </row>
-    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>145</v>
       </c>
@@ -1951,7 +1962,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:98" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>146</v>
       </c>
@@ -1965,7 +1976,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -1976,7 +1987,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>152</v>
       </c>
@@ -1996,7 +2007,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>161</v>
       </c>
@@ -2013,7 +2024,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>163</v>
       </c>
@@ -2024,7 +2035,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:98" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:98" ht="14.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>165</v>
       </c>
@@ -2038,7 +2049,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="19" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>168</v>
       </c>
@@ -2057,7 +2068,7 @@
       </c>
       <c r="AQ19" s="1"/>
     </row>
-    <row r="20" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>170</v>
       </c>
@@ -2074,7 +2085,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>180</v>
       </c>
@@ -2094,7 +2105,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>181</v>
       </c>
@@ -2112,7 +2123,7 @@
       </c>
       <c r="AM22" s="10"/>
     </row>
-    <row r="23" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>183</v>
       </c>
@@ -2144,7 +2155,7 @@
         <v>6546466555</v>
       </c>
     </row>
-    <row r="24" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -2233,7 +2244,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:98" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>194</v>
       </c>
@@ -2257,7 +2268,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:98" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:98" ht="88.3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>199</v>
       </c>
@@ -2286,7 +2297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="27" spans="1:98" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:98" ht="88.3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>214</v>
       </c>
@@ -2325,7 +2336,7 @@
       </c>
       <c r="AQ27" s="15"/>
     </row>
-    <row r="28" spans="1:98" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:98" ht="26.45" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17" t="s">
         <v>228</v>
       </c>
@@ -2387,8 +2398,8 @@
       <c r="AY28" s="17"/>
       <c r="AZ28" s="17"/>
       <c r="BA28" s="17"/>
-      <c r="BB28" s="21"/>
-      <c r="BC28" s="21"/>
+      <c r="BB28" s="22"/>
+      <c r="BC28" s="22"/>
       <c r="BD28" s="17"/>
       <c r="BE28" s="17"/>
       <c r="BF28" s="17"/>
@@ -2403,8 +2414,8 @@
       <c r="BO28" s="17"/>
       <c r="BP28" s="17"/>
       <c r="BQ28" s="17"/>
-      <c r="BR28" s="21"/>
-      <c r="BS28" s="21"/>
+      <c r="BR28" s="22"/>
+      <c r="BS28" s="22"/>
       <c r="BT28" s="17"/>
       <c r="BU28" s="17"/>
       <c r="BV28" s="17"/>
@@ -2418,35 +2429,46 @@
       <c r="CD28" s="17"/>
       <c r="CE28" s="17"/>
       <c r="CF28" s="17"/>
-      <c r="CG28" s="21"/>
-      <c r="CH28" s="21"/>
+      <c r="CG28" s="22"/>
+      <c r="CH28" s="22"/>
       <c r="CI28" s="17"/>
-      <c r="CJ28" s="21"/>
-      <c r="CK28" s="21"/>
+      <c r="CJ28" s="22"/>
+      <c r="CK28" s="22"/>
       <c r="CL28" s="17"/>
       <c r="CM28" s="17"/>
       <c r="CN28" s="17"/>
       <c r="CO28" s="17"/>
       <c r="CP28" s="17"/>
-      <c r="CQ28" s="21"/>
-      <c r="CR28" s="21"/>
-    </row>
-    <row r="30" spans="1:98" x14ac:dyDescent="0.3">
+      <c r="CQ28" s="22"/>
+      <c r="CR28" s="22"/>
+    </row>
+    <row r="29" spans="1:98" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>235</v>
+      </c>
+      <c r="AQ29" s="23" t="s">
+        <v>236</v>
+      </c>
+      <c r="AR29" s="24" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="30" spans="1:98" x14ac:dyDescent="0.35">
       <c r="CS30" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:98" x14ac:dyDescent="0.35">
       <c r="CS31" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:98" x14ac:dyDescent="0.35">
       <c r="CT32" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="12:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:24" x14ac:dyDescent="0.35">
       <c r="L33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>

</xml_diff>